<commit_message>
- support "ignored variable" via **NEW** System variable [`nexial.var.ignored`](../systemvars/index#nexial.var.ignored).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03-with-iteration.data.xlsx
+++ b/artifact/data/web-03-with-iteration.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10806"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282CD54E-79AE-A441-853E-11AB57D84FF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E497EBC9-5302-994E-81D7-E8F250B844C9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="34700" windowHeight="10500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
   <si>
     <t>true</t>
   </si>
@@ -292,7 +292,13 @@
     <t>aut : success : expected</t>
   </si>
   <si>
-    <t>1-6</t>
+    <t>B@C.org</t>
+  </si>
+  <si>
+    <t>1-7</t>
+  </si>
+  <si>
+    <t>email with invalid domain</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,35 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1516,40 +1550,40 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="48" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="50" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="47" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="49" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="46" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="45" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="44" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="43" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="45" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="44" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="41" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="40" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="39" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1560,156 +1594,156 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DC7B17-F493-C84F-A382-5EE6E86AC515}">
-  <dimension ref="A1:AAA31"/>
+  <dimension ref="A1:AAB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="31.5" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="6" width="29.5" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="51.33203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="9" max="26" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="27" max="702" width="10.83203125" style="3" collapsed="1"/>
-    <col min="703" max="703" width="10.83203125" style="3"/>
-    <col min="704" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="3" max="5" width="29.5" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="51.33203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="703" width="10.83203125" style="3" collapsed="1"/>
+    <col min="704" max="704" width="10.83203125" style="3"/>
+    <col min="705" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:702">
+    <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="GZ1" s="6"/>
-      <c r="ZZ1" s="6"/>
-    </row>
-    <row r="2" spans="1:702">
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="GZ2" s="6"/>
-      <c r="ZZ2" s="6"/>
-    </row>
-    <row r="3" spans="1:702">
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="GZ3" s="6"/>
-      <c r="ZZ3" s="6"/>
-    </row>
-    <row r="4" spans="1:702">
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="GZ4" s="6"/>
-      <c r="ZZ4" s="6"/>
-    </row>
-    <row r="5" spans="1:702">
+        <v>79</v>
+      </c>
+      <c r="HA4" s="6"/>
+      <c r="AAA4" s="6"/>
+    </row>
+    <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="GZ5" s="6"/>
-      <c r="ZZ5" s="6"/>
-    </row>
-    <row r="6" spans="1:702">
+      <c r="HA5" s="6"/>
+      <c r="AAA5" s="6"/>
+    </row>
+    <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="GZ6" s="6"/>
-      <c r="ZZ6" s="6"/>
-    </row>
-    <row r="7" spans="1:702">
+      <c r="HA6" s="6"/>
+      <c r="AAA6" s="6"/>
+    </row>
+    <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="GZ7" s="4"/>
-      <c r="ZZ7" s="5"/>
-    </row>
-    <row r="8" spans="1:702">
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="GZ8" s="4"/>
-      <c r="ZZ8" s="5"/>
-    </row>
-    <row r="9" spans="1:702">
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="GZ9" s="4"/>
-      <c r="ZZ9" s="5"/>
-    </row>
-    <row r="10" spans="1:702">
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="GZ10" s="4"/>
-      <c r="ZZ10" s="5"/>
-    </row>
-    <row r="11" spans="1:702">
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="GZ11" s="4"/>
-      <c r="ZZ11" s="5"/>
-    </row>
-    <row r="12" spans="1:702">
+      <c r="HA11" s="4"/>
+      <c r="AAA11" s="5"/>
+    </row>
+    <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="GZ12" s="4"/>
-      <c r="ZZ12" s="5"/>
-    </row>
-    <row r="13" spans="1:702">
+      <c r="HA12" s="4"/>
+      <c r="AAA12" s="5"/>
+    </row>
+    <row r="13" spans="1:703">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="GZ13" s="4"/>
-      <c r="ZZ13" s="5"/>
-    </row>
-    <row r="14" spans="1:702">
+      <c r="HA13" s="4"/>
+      <c r="AAA13" s="5"/>
+    </row>
+    <row r="14" spans="1:703">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1717,7 +1751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:702">
+    <row r="15" spans="1:703">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -1725,7 +1759,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:702">
+    <row r="16" spans="1:703">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1733,7 +1767,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -1741,7 +1775,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1749,7 +1783,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1757,7 +1791,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -1774,13 +1808,16 @@
         <v>75</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -1788,7 +1825,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -1796,7 +1833,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
@@ -1809,11 +1846,11 @@
       <c r="D23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1833,21 +1870,24 @@
         <v>67</v>
       </c>
       <c r="G24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="72">
+    <row r="26" spans="1:8" ht="72">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1864,31 +1904,34 @@
         <v>52</v>
       </c>
       <c r="F26" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="54">
+    <row r="27" spans="1:8" ht="54">
       <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="G27" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="B31" s="8"/>
     </row>
   </sheetData>
@@ -1897,149 +1940,157 @@
     <sortCondition ref="A5:A19"/>
   </sortState>
   <conditionalFormatting sqref="A22:A26 A5:A16 A28 A32:A1048576">
-    <cfRule type="beginsWith" dxfId="38" priority="42" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="40" priority="44" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A5,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="37" priority="43" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="39" priority="45" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A5,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="36" priority="44" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="46" stopIfTrue="1">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B11 B13:B16 D26 B32:B1048576 B22:B26">
-    <cfRule type="expression" dxfId="35" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="47" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="34" priority="46">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="48">
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="beginsWith" dxfId="33" priority="34" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="35" priority="36" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A17,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="32" priority="35" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="34" priority="37" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A17,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="31" priority="36" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="38" stopIfTrue="1">
       <formula>LEN(TRIM(A17))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="beginsWith" dxfId="30" priority="31" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="32" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A18,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="29" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="31" priority="34" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A18,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="33" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="35" stopIfTrue="1">
       <formula>LEN(TRIM(A18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:A21">
-    <cfRule type="beginsWith" dxfId="27" priority="28" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="29" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A19,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="28" priority="31" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A19,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="25" priority="30" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="32" stopIfTrue="1">
       <formula>LEN(TRIM(A19))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A4">
-    <cfRule type="beginsWith" dxfId="24" priority="23" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="26" priority="25" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="23" priority="24" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="25" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="22" priority="25" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="27" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B4">
-    <cfRule type="expression" dxfId="21" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="28" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="27">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="29">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="beginsWith" dxfId="19" priority="18" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="21" priority="20" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="19" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="20" priority="21" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="17" priority="20" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="22" stopIfTrue="1">
       <formula>LEN(TRIM(A27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="16" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="23" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="24">
       <formula>LEN(TRIM(C26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="beginsWith" dxfId="14" priority="13" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="16" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A29,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="15" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A29,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="15" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="17" stopIfTrue="1">
       <formula>LEN(TRIM(A29))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="expression" dxfId="11" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="18" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="17">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="19">
       <formula>LEN(TRIM(E26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="beginsWith" dxfId="9" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="11" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A31,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="10" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A31,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="12" stopIfTrue="1">
       <formula>LEN(TRIM(A31))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="6" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="14">
       <formula>LEN(TRIM(B31))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="beginsWith" dxfId="4" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="6" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A30,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="5" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A30,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="5" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26">
+    <cfRule type="expression" dxfId="3" priority="8" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="9">
+      <formula>LEN(TRIM(G26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(F26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>